<commit_message>
finished the first draft of the app!!!
</commit_message>
<xml_diff>
--- a/Outputs/Main Outputs.xlsx
+++ b/Outputs/Main Outputs.xlsx
@@ -137,16 +137,16 @@
     <t>4742495415.46458</t>
   </si>
   <si>
-    <t>81225965205.1608</t>
-  </si>
-  <si>
-    <t>7153642627.63959</t>
-  </si>
-  <si>
-    <t>75759050307.9937</t>
-  </si>
-  <si>
-    <t>-54647168.9389553</t>
+    <t>81225965205.1606</t>
+  </si>
+  <si>
+    <t>7153642627.63958</t>
+  </si>
+  <si>
+    <t>75759050307.9935</t>
+  </si>
+  <si>
+    <t>-54647168.9389555</t>
   </si>
   <si>
     <t>4664734287.7906</t>
@@ -167,16 +167,16 @@
     <t>856827778.315451</t>
   </si>
   <si>
-    <t>2374116.69826938</t>
-  </si>
-  <si>
-    <t>7215250270.56927</t>
-  </si>
-  <si>
-    <t>635453475.674464</t>
-  </si>
-  <si>
-    <t>1748335373.40218</t>
+    <t>2374116.69826937</t>
+  </si>
+  <si>
+    <t>7215250270.56926</t>
+  </si>
+  <si>
+    <t>635453475.674463</t>
+  </si>
+  <si>
+    <t>1748335373.40217</t>
   </si>
 </sst>
 </file>

</xml_diff>